<commit_message>
oferta now accepts 0 or 1
</commit_message>
<xml_diff>
--- a/public/oferta.xlsx
+++ b/public/oferta.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">subtext</t>
   </si>
   <si>
-    <t xml:space="preserve">Zamówienia przyjmujemy do 15.04.2025 r. Odbiór: 18.04.2025 r. 9:30–18:00.</t>
+    <t xml:space="preserve">Zamów dania na święta z odbiorem w barze. Przyjmujemy zamówienia do 15.04.2025 r., odbiór 18.04.2025 r. w godz. 9:30–18:00.</t>
   </si>
   <si>
     <t xml:space="preserve">Biała kiełbasa</t>
@@ -143,9 +143,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -213,16 +212,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,8 +428,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>